<commit_message>
fixed a couple tests
</commit_message>
<xml_diff>
--- a/adios_db/adios_db/test/test_importing/example_data/LSU_AlaskaNorthSlope.xlsx
+++ b/adios_db/adios_db/test/test_importing/example_data/LSU_AlaskaNorthSlope.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/adios_db/test/test_importing/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{CD5082A6-4706-BF44-89DA-702026BD329B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C3392-0C63-8E49-8C33-98EA0C97405B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="1500" windowWidth="29500" windowHeight="16780" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="3400" yWindow="2000" windowWidth="21240" windowHeight="11740" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="LSU_AlaskaNorthSlope" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,8 @@
     <author>tc={EC1C01C4-654C-344B-9568-9DE6B90917FC}</author>
     <author>tc={C79285D1-5B02-454C-A1B4-F58D5EAD35F8}</author>
     <author>tc={9FEE7A33-6DDA-7941-9C9C-86088633A24E}</author>
-    <author>tc={D7A222A2-D0E2-D148-8CB1-9330E946D93D}</author>
-    <author>tc={E7564FA4-067F-C44F-8A96-1B440CB95A7C}</author>
     <author>tc={059E4DD8-F1D3-EE45-8585-CC72603E1B73}</author>
-    <author>tc={B24D8019-6307-814D-8C62-B2C5B2CCBDE1}</author>
     <author>tc={238543C2-308B-524A-B991-946508025E21}</author>
-    <author>tc={038C3DF9-268E-EA4A-A3AE-0FA78D07ADDD}</author>
   </authors>
   <commentList>
     <comment ref="B8" authorId="0" shapeId="0" xr:uid="{EC1C01C4-654C-344B-9568-9DE6B90917FC}">
@@ -184,7 +180,70 @@
         </r>
       </text>
     </comment>
-    <comment ref="A37" authorId="3" shapeId="0" xr:uid="{D7A222A2-D0E2-D148-8CB1-9330E946D93D}">
+    <comment ref="A70" authorId="3" shapeId="0" xr:uid="{059E4DD8-F1D3-EE45-8585-CC72603E1B73}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Comment:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    Chris said not to make a separate spreadsheet for other subsamples under the same record. He said to copy and paste everything under “Subsample metadata” on the same spreadsheet and fill in the fields with the new information.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A92" authorId="4" shapeId="0" xr:uid="{238543C2-308B-524A-B991-946508025E21}">
       <text>
         <r>
           <rPr>
@@ -201,97 +260,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B37" authorId="4" shapeId="0" xr:uid="{E7564FA4-067F-C44F-8A96-1B440CB95A7C}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Initially “Viscosity” was in cell B32 and “Unit” was in cell C32. However, the drop down ,its of units was in cell B33 and it would not let me type in the viscosity value, so I switched their placements with one another, just FYI</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A71" authorId="5" shapeId="0" xr:uid="{059E4DD8-F1D3-EE45-8585-CC72603E1B73}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Chris said not to make a separate spreadsheet for other subsamples under the same record. He said to copy and paste everything under “Subsample metadata” on the same spreadsheet and fill in the fields with the new information.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B88" authorId="6" shapeId="0" xr:uid="{B24D8019-6307-814D-8C62-B2C5B2CCBDE1}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Initially “Viscosity” was in cell B32 and “Unit” was in cell C32. However, the drop down ,its of units was in cell B33 and it would not let me type in the viscosity value, so I switched their placements with one another, just FYI</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A93" authorId="7" shapeId="0" xr:uid="{238543C2-308B-524A-B991-946508025E21}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    I had to add all of this manually, we need a dynamic viscosity place… these values are in cP not cSt so there is no option for that with the kinematic pro down list</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B93" authorId="8" shapeId="0" xr:uid="{038C3DF9-268E-EA4A-A3AE-0FA78D07ADDD}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Initially “Viscosity” was in cell B32 and “Unit” was in cell C32. However, the drop down ,its of units was in cell B33 and it would not let me type in the viscosity value, so I switched their placements with one another, just FYI</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="161">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -765,9 +739,6 @@
     </r>
   </si>
   <si>
-    <t>30.5% Weathered Oil</t>
-  </si>
-  <si>
     <t>ANS</t>
   </si>
   <si>
@@ -777,9 +748,6 @@
     <t>Alaska, USA</t>
   </si>
   <si>
-    <t>Just a little bit of text.'</t>
-  </si>
-  <si>
     <t>Original fresh oil sample</t>
   </si>
   <si>
@@ -790,6 +758,15 @@
   </si>
   <si>
     <t>Just a little bit of text.</t>
+  </si>
+  <si>
+    <t>30% Evaporated</t>
+  </si>
+  <si>
+    <t>30.5% Evaporated (lab weathered)</t>
+  </si>
+  <si>
+    <t>Weathered in the lab by unknown protocol</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1225,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38:C39"/>
+    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1270,7 +1247,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1296,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1304,7 +1281,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1377,7 +1354,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1385,7 +1362,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1393,7 +1370,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1401,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1559,122 +1536,121 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B37" s="9" t="s">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
+      <c r="A38" t="s">
         <v>23</v>
       </c>
-      <c r="B38" s="13">
+      <c r="B38">
         <v>11.5</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38">
         <v>15</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
+      <c r="A39" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="13">
+      <c r="B39">
         <v>23.2</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" t="s">
         <v>73</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39">
         <v>0</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="9"/>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>24</v>
+      <c r="A42" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C46" t="s">
-        <v>75</v>
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E47" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E48" t="s">
         <v>56</v>
@@ -1682,34 +1658,34 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" t="s">
-        <v>56</v>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>29</v>
+      </c>
+      <c r="C51" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B52" t="s">
-        <v>29</v>
+      <c r="A52" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C52" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C53" t="s">
         <v>75</v>
@@ -1717,7 +1693,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" t="s">
         <v>75</v>
@@ -1725,54 +1701,57 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" t="s">
+        <v>30</v>
+      </c>
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" t="s">
+        <v>46</v>
+      </c>
+      <c r="G59" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C60" t="s">
-        <v>47</v>
-      </c>
-      <c r="D60" t="s">
-        <v>30</v>
-      </c>
       <c r="E60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" t="s">
-        <v>46</v>
-      </c>
-      <c r="G60" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
       <c r="D61" t="s">
         <v>75</v>
@@ -1782,48 +1761,48 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" t="s">
+        <v>49</v>
+      </c>
+      <c r="F63" t="s">
+        <v>46</v>
+      </c>
+      <c r="G63" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A64" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="12">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D64" t="s">
         <v>75</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E64" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C64" t="s">
-        <v>47</v>
-      </c>
-      <c r="D64" t="s">
-        <v>30</v>
-      </c>
-      <c r="E64" t="s">
-        <v>49</v>
-      </c>
-      <c r="F64" t="s">
-        <v>46</v>
-      </c>
-      <c r="G64" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C65" s="12">
-        <v>1.1100000000000001</v>
+        <v>137</v>
       </c>
       <c r="D65" t="s">
         <v>75</v>
@@ -1832,207 +1811,192 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D66" t="s">
-        <v>75</v>
-      </c>
-      <c r="E66" t="s">
-        <v>74</v>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B67" t="s">
+        <v>45</v>
+      </c>
+      <c r="C67" t="s">
+        <v>61</v>
+      </c>
+      <c r="D67" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" t="s">
+        <v>49</v>
+      </c>
+      <c r="F67" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B68" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" t="s">
-        <v>61</v>
+      <c r="A68" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="D68" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>49</v>
-      </c>
-      <c r="F68" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D69" t="s">
-        <v>141</v>
-      </c>
-      <c r="E69" t="s">
         <v>140</v>
       </c>
     </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
-        <v>16</v>
+      <c r="A71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="12" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="C73" t="s">
-        <v>152</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>155</v>
+        <v>15</v>
+      </c>
+      <c r="C75">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="D75" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76">
-        <v>3.4000000000000002E-2</v>
+        <v>14</v>
       </c>
       <c r="D76" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>14</v>
-      </c>
-      <c r="B77">
-        <v>150</v>
-      </c>
-      <c r="C77">
-        <v>250</v>
-      </c>
-      <c r="D77" t="s">
         <v>57</v>
       </c>
     </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B78" t="s">
+        <v>59</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B79" t="s">
-        <v>59</v>
-      </c>
-      <c r="C79" t="s">
-        <v>61</v>
-      </c>
-      <c r="D79" t="s">
-        <v>60</v>
+      <c r="A79" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="13">
+        <v>-6</v>
+      </c>
+      <c r="D79" s="13"/>
+      <c r="E79" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C80" s="13">
-        <v>-6</v>
+        <v>115</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>26</v>
-      </c>
-      <c r="C81" s="13">
-        <v>115</v>
-      </c>
-      <c r="D81" s="13"/>
-      <c r="E81" t="s">
-        <v>57</v>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>27</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" t="s">
+        <v>31</v>
+      </c>
+      <c r="E82" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>27</v>
-      </c>
-      <c r="B83" t="s">
-        <v>54</v>
-      </c>
-      <c r="C83" t="s">
-        <v>63</v>
-      </c>
-      <c r="D83" t="s">
-        <v>31</v>
-      </c>
-      <c r="E83" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B83" s="13">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="C83" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D83" s="13">
+        <v>15</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>18</v>
       </c>
-      <c r="B84" s="13">
-        <v>0.93400000000000005</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D84" s="13">
-        <v>15</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>18</v>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>55</v>
+      </c>
+      <c r="B87" t="s">
+        <v>36</v>
+      </c>
+      <c r="C87" t="s">
+        <v>63</v>
+      </c>
+      <c r="D87" t="s">
+        <v>31</v>
+      </c>
+      <c r="E87" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B88" t="s">
-        <v>63</v>
-      </c>
-      <c r="C88" t="s">
-        <v>36</v>
-      </c>
-      <c r="D88" t="s">
-        <v>31</v>
-      </c>
-      <c r="E88" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
@@ -2045,163 +2009,165 @@
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
-        <v>23</v>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C92" t="s">
+        <v>63</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C93" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>63</v>
+        <v>23</v>
+      </c>
+      <c r="B93" s="13">
+        <v>625</v>
+      </c>
+      <c r="C93" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D93" s="13">
+        <v>15</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="13">
+        <v>4230</v>
+      </c>
+      <c r="C94" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="13">
-        <v>625</v>
-      </c>
       <c r="D94" s="13">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E94" s="13" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A95" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B95" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C95" s="13">
-        <v>4230</v>
-      </c>
-      <c r="D95" s="13">
-        <v>0</v>
-      </c>
-      <c r="E95" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A96" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
+      <c r="A96" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>24</v>
+      <c r="A98" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="B99" t="s">
+        <v>62</v>
+      </c>
+      <c r="C99" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>19</v>
+        <v>37</v>
+      </c>
+      <c r="B100" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B101" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C101" t="s">
-        <v>57</v>
+        <v>30</v>
+      </c>
+      <c r="D101" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>37</v>
-      </c>
-      <c r="B102" t="s">
-        <v>47</v>
-      </c>
-      <c r="C102" t="s">
-        <v>75</v>
+        <v>21</v>
+      </c>
+      <c r="E102" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>34</v>
-      </c>
-      <c r="B103" t="s">
-        <v>29</v>
-      </c>
-      <c r="C103" t="s">
-        <v>30</v>
-      </c>
-      <c r="D103" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E103" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E104" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E105" t="s">
-        <v>56</v>
-      </c>
-    </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" t="s">
-        <v>28</v>
-      </c>
-      <c r="E106" t="s">
-        <v>56</v>
+      <c r="A106" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B106" t="s">
+        <v>29</v>
+      </c>
+      <c r="C106" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C107" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B108" t="s">
-        <v>29</v>
+      <c r="A108" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C108" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C109" t="s">
         <v>75</v>
@@ -2209,154 +2175,138 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C110" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C111" t="s">
-        <v>75</v>
-      </c>
+      <c r="A111" s="2"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B114" t="s">
+        <v>45</v>
+      </c>
+      <c r="C114" t="s">
+        <v>47</v>
+      </c>
+      <c r="D114" t="s">
+        <v>30</v>
+      </c>
+      <c r="E114" t="s">
+        <v>49</v>
+      </c>
+      <c r="F114" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D115" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="2"/>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>19</v>
+      <c r="E115" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B116" t="s">
+      <c r="A116" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D116" t="s">
+        <v>75</v>
+      </c>
+      <c r="E116" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B118" t="s">
         <v>45</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C118" t="s">
         <v>47</v>
       </c>
-      <c r="D116" t="s">
+      <c r="D118" t="s">
         <v>30</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E118" t="s">
         <v>49</v>
       </c>
-      <c r="F116" t="s">
+      <c r="F118" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D117" t="s">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C119" s="13">
+        <v>1.5</v>
+      </c>
+      <c r="D119" t="s">
         <v>75</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E119" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D118" t="s">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D120" t="s">
         <v>75</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E120" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="2"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B120" t="s">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B122" t="s">
         <v>45</v>
       </c>
-      <c r="C120" t="s">
-        <v>47</v>
-      </c>
-      <c r="D120" t="s">
-        <v>30</v>
-      </c>
-      <c r="E120" t="s">
+      <c r="C122" t="s">
+        <v>61</v>
+      </c>
+      <c r="D122" t="s">
+        <v>134</v>
+      </c>
+      <c r="E122" t="s">
         <v>49</v>
       </c>
-      <c r="F120" t="s">
+      <c r="F122" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C121" s="13">
-        <v>1.5</v>
-      </c>
-      <c r="D121" t="s">
-        <v>75</v>
-      </c>
-      <c r="E121" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D122" t="s">
-        <v>75</v>
-      </c>
-      <c r="E122" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B124" t="s">
-        <v>45</v>
-      </c>
-      <c r="C124" t="s">
-        <v>61</v>
-      </c>
-      <c r="D124" t="s">
-        <v>134</v>
-      </c>
-      <c r="E124" t="s">
-        <v>49</v>
-      </c>
-      <c r="F124" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="2" t="s">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="D125" t="s">
+      <c r="D123" t="s">
         <v>141</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E123" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2370,31 +2320,31 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$6:$B$8</xm:f>
           </x14:formula1>
-          <xm:sqref>E24:E25 E28:E30 D21 E48:E50 C45 E33:E36 E38:E40 E80:E81 E84:E86 D77 E104:E106 C101 E89:E92 E94:E96</xm:sqref>
+          <xm:sqref>E24:E25 E28:E30 D21 E47:E49 C44 E33:E36 E79:E80 E83:E85 D76 E102:E104 C99 E88:E91 E93:E94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1033A37D-2D0D-F04D-9BEA-7F24863237D0}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$C$6:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>C28:C30 C84:C86</xm:sqref>
+          <xm:sqref>C28:C30 C83:C85</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BD19B16E-3F59-184B-ACC0-71023DB30176}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$D$6:$D$8</xm:f>
           </x14:formula1>
-          <xm:sqref>B89</xm:sqref>
+          <xm:sqref>C88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4FE116B8-5867-7C4D-BE9F-83D0035A698F}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$6:$F$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C53:C56 C48:C50 C46 D20 D61:D62 D65:D66 C109:C112 C104:C106 C102 D76 D117:D118 D121:D122</xm:sqref>
+          <xm:sqref>C52:C55 C47:C49 C45 D20 D60:D61 D64:D65 C107:C110 C102:C104 C100 D75 D115:D116 D119:D120</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0BDD9F5B-C4F1-C24B-AF14-33A5AF4296F8}">
           <x14:formula1>
             <xm:f>'Pick List Data'!$F$5:$G$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B43 B20 E61:E62 E65:E66 B99 B76 E117:E118 E121:E122</xm:sqref>
+          <xm:sqref>B42 B20 E60:E61 E64:E65 B97 B75 E115:E116 E119:E120</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{21D6D9B9-727A-8848-9369-CAA47CDDF88B}">
           <x14:formula1>
@@ -2412,7 +2362,7 @@
           <x14:formula1>
             <xm:f>'Pick List Data'!$B$5:$H$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E69 E125</xm:sqref>
+          <xm:sqref>E68 E123</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
added code to read multiple subsammples
</commit_message>
<xml_diff>
--- a/adios_db/adios_db/test/test_importing/example_data/LSU_AlaskaNorthSlope.xlsx
+++ b/adios_db/adios_db/test/test_importing/example_data/LSU_AlaskaNorthSlope.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris.barker/Hazmat/GitLab/oil_database/adios_db/adios_db/test/test_importing/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7C3392-0C63-8E49-8C33-98EA0C97405B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665ACEF2-583F-6340-832B-ED39BC44426B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="2000" windowWidth="21240" windowHeight="11740" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
+    <workbookView xWindow="21160" yWindow="4180" windowWidth="25200" windowHeight="19020" xr2:uid="{A4891382-C4C2-C649-BC90-83075B8F427D}"/>
   </bookViews>
   <sheets>
     <sheet name="LSU_AlaskaNorthSlope" sheetId="1" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="162">
   <si>
     <t>ADIOS Data Model Version</t>
   </si>
@@ -673,9 +673,6 @@
   </si>
   <si>
     <t xml:space="preserve">  compound 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Sulphur</t>
   </si>
   <si>
     <t xml:space="preserve">  Composition 2</t>
@@ -767,6 +764,12 @@
   </si>
   <si>
     <t>Weathered in the lab by unknown protocol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Composition 1</t>
+  </si>
+  <si>
+    <t>Sulfur Content</t>
   </si>
 </sst>
 </file>
@@ -1227,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1AE41B5-EBD4-784F-86F2-E9CEA1F05E22}">
   <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1247,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1260,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1273,7 +1276,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1281,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1292,7 +1295,7 @@
         <v>2011</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1341,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1354,7 +1357,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,7 +1365,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1370,7 +1373,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1378,7 +1381,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1788,11 +1791,12 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C64" s="12">
-        <v>1.1100000000000001</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="B64" t="s">
+        <v>161</v>
+      </c>
+      <c r="C64" s="12"/>
       <c r="D64" t="s">
         <v>75</v>
       </c>
@@ -1802,7 +1806,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D65" t="s">
         <v>75</v>
@@ -1813,7 +1817,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B67" t="s">
         <v>45</v>
@@ -1833,13 +1837,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D68" t="s">
+        <v>140</v>
+      </c>
+      <c r="E68" t="s">
         <v>139</v>
-      </c>
-      <c r="D68" t="s">
-        <v>141</v>
-      </c>
-      <c r="E68" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -1852,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -1860,7 +1864,7 @@
         <v>10</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -1873,7 +1877,7 @@
         <v>11</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2011,7 +2015,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B92" s="9" t="s">
         <v>36</v>
@@ -2256,9 +2260,12 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C119" s="13">
+        <v>160</v>
+      </c>
+      <c r="B119" t="s">
+        <v>161</v>
+      </c>
+      <c r="C119" s="12">
         <v>1.5</v>
       </c>
       <c r="D119" t="s">
@@ -2270,7 +2277,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D120" t="s">
         <v>75</v>
@@ -2281,7 +2288,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B122" t="s">
         <v>45</v>
@@ -2301,13 +2308,13 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D123" t="s">
+        <v>140</v>
+      </c>
+      <c r="E123" t="s">
         <v>139</v>
-      </c>
-      <c r="D123" t="s">
-        <v>141</v>
-      </c>
-      <c r="E123" t="s">
-        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2420,7 +2427,7 @@
         <v>80</v>
       </c>
       <c r="H5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
@@ -2446,7 +2453,7 @@
         <v>47</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
@@ -2469,7 +2476,7 @@
         <v>75</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
@@ -2492,7 +2499,7 @@
         <v>81</v>
       </c>
       <c r="H8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
@@ -2503,7 +2510,7 @@
         <v>76</v>
       </c>
       <c r="H9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
@@ -2511,7 +2518,7 @@
         <v>78</v>
       </c>
       <c r="H10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
@@ -2519,7 +2526,7 @@
         <v>79</v>
       </c>
       <c r="H11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.2">

</xml_diff>